<commit_message>
Added initial WebUI project
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebie\Desktop\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0053EFAB-651D-413B-99BF-10DCE11CC7C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0984F4-BC01-4246-90C3-BC5B92C758BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Meeting und Anpassungen für das Wireframe</t>
+  </si>
+  <si>
+    <t>Passendes UI-Framework rausgesucht</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,153 +604,162 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44168</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on the WebUI
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECDD6AE-15EA-4688-B09F-E7676D1F8FC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A104D-FA3A-42AB-8A1B-5AC513D51EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13815" yWindow="1590" windowWidth="13545" windowHeight="9285" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Passendes UI-Framework rausgesucht</t>
+  </si>
+  <si>
+    <t>Dokus und Tutorials über Vue.js gelesen/gesehen</t>
+  </si>
+  <si>
+    <t>Meeting + WebUI</t>
   </si>
 </sst>
 </file>
@@ -460,7 +466,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,147 +625,174 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>44174</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>44182</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>44183</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
       <c r="C14">
         <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added development project for WebUI to git
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D890585-4A08-49E2-A964-96DE7C87B0ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AAD28D-90AC-4888-84F0-D6815DB4F89B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,118 +702,127 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>44218</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated stundenliste and worked on WebUI
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AAD28D-90AC-4888-84F0-D6815DB4F89B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AC96C2-0435-408D-94B1-8B4C9471E4E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,11 +707,11 @@
         <v>44218</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
@@ -720,109 +720,109 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrated SASS in WebUI
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AC96C2-0435-408D-94B1-8B4C9471E4E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAA45E9-6BC2-4FC2-BE81-4F7C779C83D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Datum</t>
   </si>
@@ -469,7 +469,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,111 +718,120 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>44221</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updated responsive design of WebUI.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B98D50B-616C-4B02-814B-2B49E0096E6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEB591B-E4BF-4D7B-B695-E445FC8208EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="2220" windowWidth="17070" windowHeight="11790" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Meeting + Development WebUI</t>
+  </si>
+  <si>
+    <t>Meeting+Development WebUI</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,99 +754,108 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>44245</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Channel.vue to work properly with modals. Updated the logo and favicon.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC3B8FD-1A95-4780-BDCE-9D6783F1BA6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCED4D2B-C601-4A3F-BF35-8603F727BF8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Datum</t>
   </si>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,93 +769,102 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>44246</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added local files for bootstrap and fontawesome instead of using CDNs for them. Added apexcharts to WebUI for data visualization.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCED4D2B-C601-4A3F-BF35-8603F727BF8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768D2CD6-45AD-4FA8-83B6-BFF700BCEA21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,11 +773,11 @@
         <v>44246</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -786,85 +786,85 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Research on apexcharts. - Put apexchart reference in Channel.vue instead of main.js
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768D2CD6-45AD-4FA8-83B6-BFF700BCEA21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371C5605-56C5-4498-9154-7ECAA76947B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Meeting+Development WebUI</t>
+  </si>
+  <si>
+    <t>Meeting+Investigating Apexcharts</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,87 +787,105 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>44247</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>44250</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added custom zooming to apexchart
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\GitHub\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371C5605-56C5-4498-9154-7ECAA76947B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C6D8CC-C3A4-4E3E-8B77-964F84D71F80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Datum</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Meeting+Investigating Apexcharts</t>
+  </si>
+  <si>
+    <t>Poster + Development WebUI</t>
+  </si>
+  <si>
+    <t>29.02.2021</t>
+  </si>
+  <si>
+    <t>Research on alternatives for apexcharts</t>
+  </si>
+  <si>
+    <t>Research on custom range sliders + Development WebUI</t>
   </si>
 </sst>
 </file>
@@ -475,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,75 +829,118 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>44251</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>95</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>44252</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>102</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>44253</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>44254</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>118</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>44255</v>
+      </c>
+      <c r="B28">
+        <v>7</v>
+      </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>134</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>44256</v>
+      </c>
+      <c r="B30">
+        <v>8</v>
+      </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>142</v>
+      </c>
+      <c r="D30" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C31">
-        <f t="shared" si="0"/>
-        <v>90</v>
+      <c r="A31" s="4">
+        <v>44257</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C32">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34">
-        <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <f t="shared" si="0"/>
-        <v>90</v>
+      <c r="A32" s="4">
+        <v>44258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- installed jquery-ui - rearranged some files
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8039983E-E895-446D-A045-E20C4432DC4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D348D7F-5904-4D26-AF28-04DDC7A40FAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Datum</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Studenliste von Sebastian Ederer</t>
+  </si>
+  <si>
+    <t>Fixed git-merging issues</t>
+  </si>
+  <si>
+    <t>Organizational stuff; Research on jquery-ui</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,198 +502,214 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4">
+        <v>44276</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
       <c r="C5">
         <f>B5</f>
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4">
+        <v>44291</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
       <c r="C6">
         <f>C5+B6</f>
-        <v>0</v>
+        <v>6.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="C7">
         <f t="shared" ref="C7:C30" si="0">C6+B7</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8">
         <f>C7+B8</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added touch support to apexchart-scrollbar - fixed bug in the productive versions routing
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40886559-B613-4952-842A-34202FDDF111}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C9EBAE-445C-45EB-B800-C0157F87A7B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Datum</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Implemented Zooming-Feature with jquery-ui; Implemented vue-routing</t>
+  </si>
+  <si>
+    <t>Meeting + css fix</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,170 +571,178 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4">
+        <v>44308</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- started to implement funktionality to receive data
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD6CC82-0F0B-46AE-AA85-EB6E81F237B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695ABD79-2037-42C6-9C10-3E5FF72F8926}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>Added touch-support for jquery ui, fixed routing and merge issues</t>
   </si>
   <si>
-    <t>Fixed vue routing</t>
+    <t>Fixed vue routing; started to implement data receiving</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,11 +629,11 @@
         <v>44318</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -643,139 +643,139 @@
       <c r="A13" s="4"/>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- worked on UplutChart component
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA776155-7C6C-4BFE-92F9-FBEE60B5C5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C173F5-EE25-4B38-B3D6-0E9BDFC0975F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Datum</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Worked on uPlot; Meeting</t>
+  </si>
+  <si>
+    <t>Bug fixing; Research and working on uPlot and data visualization</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,121 +697,129 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4">
+        <v>44351</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- started to implement zooming for uplot charts.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C173F5-EE25-4B38-B3D6-0E9BDFC0975F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB74D111-EFDB-459A-9215-A1B5A2ADECED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Bug fixing; Research and working on uPlot and data visualization</t>
+  </si>
+  <si>
+    <t>Implemented zooming for uPlot.</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,115 +714,123 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>44354</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- experimenting with UI/UX
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AA87D9-048B-47EE-938C-9FD1B440147F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CF4E9A-7F5A-454B-8A8C-B98FA8EF5722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>Meeting + implemented conditional rendering for data annotations</t>
+  </si>
+  <si>
+    <t>Improved data annotations. Started to improve navigation of charts</t>
+  </si>
+  <si>
+    <t>Research on canvas and experimenting mit UI/UX design.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,79 +809,95 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4">
+        <v>44413</v>
+      </c>
+      <c r="B22" s="5">
+        <v>6</v>
+      </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="4">
+        <v>44428</v>
+      </c>
+      <c r="B23" s="5">
+        <v>7</v>
+      </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implemented chart navigation
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CF4E9A-7F5A-454B-8A8C-B98FA8EF5722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E837C715-EB37-4DFD-B19D-DCEA15B828A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Datum</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Research on canvas and experimenting mit UI/UX design.</t>
+  </si>
+  <si>
+    <t>Research on UI/UX for chart navigation</t>
+  </si>
+  <si>
+    <t>Further implemented chart navigation</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,65 +845,89 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4">
+        <v>44433</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="4">
+        <v>44442</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4</v>
+      </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="4">
+        <v>44443</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3</v>
+      </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31">
         <f>C30+B31</f>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: worked on decoded data.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3A1260-EF63-4CB6-92E6-8BCBB0774AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A4614-93D7-43E7-B90C-73A04D4F2AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Datum</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Chart navigation (mobile support)</t>
+  </si>
+  <si>
+    <t>Videoaufnahme, bug fixing</t>
+  </si>
+  <si>
+    <t>Poster</t>
   </si>
 </sst>
 </file>
@@ -511,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,24 +947,40 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4">
+        <v>44452</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="4">
+        <v>44456</v>
+      </c>
+      <c r="B31" s="5">
+        <v>4</v>
+      </c>
       <c r="C31">
         <f>C30+B31</f>
-        <v>119</v>
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="C32">
         <f>C31+B32</f>
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated stundenliste, removed dblclick event from channel name
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-SebastianEderer.xlsx
+++ b/stundenlisten/Stundenliste-SebastianEderer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Studium\PA1\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC248D-3CFE-41B6-AC16-F408BB654E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F216C6-CBE3-44C7-B907-76ECEE4591DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Datum</t>
   </si>
@@ -132,7 +132,10 @@
     <t>Poster</t>
   </si>
   <si>
-    <t xml:space="preserve">Implemented DecodedData list with dropdown. </t>
+    <t xml:space="preserve">Implemented DecodedData list with dropdown, fixed DataAnnotations, disabled default zooming, synced cursors between all charts </t>
+  </si>
+  <si>
+    <t>Präsentation</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,6 +207,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -518,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBE639EC-E41E-4FE7-B5F2-AD1BA98AEA4D}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,14 +988,29 @@
         <v>44457</v>
       </c>
       <c r="B32" s="5">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <f>C31+B32</f>
-        <v>126.5</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>44457</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <f>C32+B33</f>
+        <v>130</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>